<commit_message>
Most of tasks done
</commit_message>
<xml_diff>
--- a/Sources_Database.xlsx
+++ b/Sources_Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin barcenas\Downloads\MAYALEX_Workflow\MAYALEX_Workflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\MAYALEX Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7188F587-CD01-435C-87EE-288F8CC1BC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1256743-2051-4D23-BEF8-FCA6DCE4F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>@book{robertson2010colonial,&lt;br&gt; author = {Robertson, J. and Law, D. and Haertel, R.},&lt;br&gt; title = {Colonial Ch'olti': The seventeenth century Morán Manuscript},&lt;br&gt; year = {2010},&lt;br&gt; publisher = {University of Oklahoma Press},&lt;br&gt; address = {Norman, OK}&lt;br&gt;}</t>
+  </si>
+  <si>
+    <t>@manuscript{calipino_motul,&lt;br&gt; title = {Calipino de Motul},&lt;br&gt; note = {Manuscript, page 1r}&lt;br&gt;}</t>
+  </si>
+  <si>
+    <t>@manuscript{vocabulario_kiche,&lt;br&gt; title = {El Vocabulario K'iche' Otlateca},&lt;br&gt; pages = {38r}&lt;br&gt;}</t>
+  </si>
+  <si>
+    <t>"@book{coto1983,&lt;br&gt;  author = {Coto},&lt;br&gt;  title = {Coto Manuscript},&lt;br&gt;  year = {1983},&lt;br&gt;  note = {Original manuscript from 1656},&lt;br&gt;  pages = {277}&lt;br&gt;}{coto1983,&lt;br&gt; author = {Coto},&lt;br&gt; title = {Coto Manuscript},&lt;br&gt; year = {1983},&lt;br&gt; note = {Original manuscript from 1656}&lt;br&gt;}"</t>
   </si>
 </sst>
 </file>
@@ -468,22 +477,22 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7265625" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,7 +518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -535,7 +544,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -554,8 +563,14 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -581,7 +596,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -600,14 +615,14 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>384</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -626,8 +641,14 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -645,6 +666,12 @@
       </c>
       <c r="F7" t="s">
         <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most of the tasks done missing spn eng check for pos in kauf:
</commit_message>
<xml_diff>
--- a/Sources_Database.xlsx
+++ b/Sources_Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\MAYALEX Workflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin barcenas\Downloads\MAYALEX_Workflow\MAYALEX_Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1256743-2051-4D23-BEF8-FCA6DCE4F593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821612F-C49C-4998-83C2-30257503AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
   <si>
     <t>Abbreviation</t>
   </si>
   <si>
-    <t>Source Name</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Pages</t>
   </si>
   <si>
-    <t>CM</t>
-  </si>
-  <si>
     <t>FAMSI</t>
   </si>
   <si>
@@ -68,30 +62,12 @@
     <t>VKO</t>
   </si>
   <si>
-    <t>Coto</t>
-  </si>
-  <si>
-    <t>Preliminary Mayan Etymological Dictionary</t>
-  </si>
-  <si>
     <t>Terrence Kaufman, John Justeson</t>
   </si>
   <si>
     <t>A Preliminary Mayan Etymological Dictionary</t>
   </si>
   <si>
-    <t>Calipino de Motul</t>
-  </si>
-  <si>
-    <t>Foundation for the Advancement of Mesoamerican Studies</t>
-  </si>
-  <si>
-    <t>Colonial Ch'olti' Manuscript</t>
-  </si>
-  <si>
-    <t>Vocabulario K'iche' Otlateca</t>
-  </si>
-  <si>
     <t>Coto Manuscript</t>
   </si>
   <si>
@@ -137,23 +113,241 @@
     <t>@book{robertson2010colonial,&lt;br&gt; author = {Robertson, J. and Law, D. and Haertel, R.},&lt;br&gt; title = {Colonial Ch'olti': The seventeenth century Morán Manuscript},&lt;br&gt; year = {2010},&lt;br&gt; publisher = {University of Oklahoma Press},&lt;br&gt; address = {Norman, OK}&lt;br&gt;}</t>
   </si>
   <si>
-    <t>@manuscript{calipino_motul,&lt;br&gt; title = {Calipino de Motul},&lt;br&gt; note = {Manuscript, page 1r}&lt;br&gt;}</t>
-  </si>
-  <si>
     <t>@manuscript{vocabulario_kiche,&lt;br&gt; title = {El Vocabulario K'iche' Otlateca},&lt;br&gt; pages = {38r}&lt;br&gt;}</t>
   </si>
   <si>
     <t>"@book{coto1983,&lt;br&gt;  author = {Coto},&lt;br&gt;  title = {Coto Manuscript},&lt;br&gt;  year = {1983},&lt;br&gt;  note = {Original manuscript from 1656},&lt;br&gt;  pages = {277}&lt;br&gt;}{coto1983,&lt;br&gt; author = {Coto},&lt;br&gt; title = {Coto Manuscript},&lt;br&gt; year = {1983},&lt;br&gt; note = {Original manuscript from 1656}&lt;br&gt;}"</t>
+  </si>
+  <si>
+    <t>FAMSI Sources</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>Beltrán</t>
+  </si>
+  <si>
+    <t>Buenaventura</t>
+  </si>
+  <si>
+    <t>Coronel</t>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>Cordemex</t>
+  </si>
+  <si>
+    <t>Roys</t>
+  </si>
+  <si>
+    <t>Swadish</t>
+  </si>
+  <si>
+    <t>Herrera</t>
+  </si>
+  <si>
+    <t>Juan Pío Pérez</t>
+  </si>
+  <si>
+    <t>Barrera</t>
+  </si>
+  <si>
+    <t>Nikolai Grube</t>
+  </si>
+  <si>
+    <t>Motul</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Ticul</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Beltrán’s Arte</t>
+  </si>
+  <si>
+    <t>Buenaventura’s Arte</t>
+  </si>
+  <si>
+    <t>Coronel’s Arte</t>
+  </si>
+  <si>
+    <t>David Bolles entries</t>
+  </si>
+  <si>
+    <t>David Bolles English-Mayan</t>
+  </si>
+  <si>
+    <t>David Bolles Mayan-English</t>
+  </si>
+  <si>
+    <t>Pérez 1898</t>
+  </si>
+  <si>
+    <t>Cordemex Mayan-Spanish</t>
+  </si>
+  <si>
+    <t>Cordemex Spanish-Mayan</t>
+  </si>
+  <si>
+    <t>Roys Latin-Mayan</t>
+  </si>
+  <si>
+    <t>Roys Mayan-Latin</t>
+  </si>
+  <si>
+    <t>Swadish Mayan-Spanish</t>
+  </si>
+  <si>
+    <t>Swadish Spanish-Mayan</t>
+  </si>
+  <si>
+    <t>Herrera Mayan-Spanish</t>
+  </si>
+  <si>
+    <t>Juan Pío Pérez’s Diccionario</t>
+  </si>
+  <si>
+    <t>Barrera Latin-Mayan</t>
+  </si>
+  <si>
+    <t>Barrera Mayan-Latin</t>
+  </si>
+  <si>
+    <t>Motul Mayan-Spanish</t>
+  </si>
+  <si>
+    <t>Motul Spanish-Mayan</t>
+  </si>
+  <si>
+    <t>San Francisco Mayan-Spanish</t>
+  </si>
+  <si>
+    <t>San Francisco Spanish-Mayan</t>
+  </si>
+  <si>
+    <t>Diccionario de Ticul, published 1898</t>
+  </si>
+  <si>
+    <t>Vienna Spanish-Mayan</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>BUE</t>
+  </si>
+  <si>
+    <t>COR</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>DBM</t>
+  </si>
+  <si>
+    <t>DBE</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>CRS</t>
+  </si>
+  <si>
+    <t>EBL</t>
+  </si>
+  <si>
+    <t>EBM</t>
+  </si>
+  <si>
+    <t>EMM</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>HER</t>
+  </si>
+  <si>
+    <t>JPP</t>
+  </si>
+  <si>
+    <t>NEL</t>
+  </si>
+  <si>
+    <t>NEM</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>MTM</t>
+  </si>
+  <si>
+    <t>MTS</t>
+  </si>
+  <si>
+    <t>SFM</t>
+  </si>
+  <si>
+    <t>SFS</t>
+  </si>
+  <si>
+    <t>TIC</t>
+  </si>
+  <si>
+    <t>VNS</t>
+  </si>
+  <si>
+    <t>COT</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>http://www.famsi.org/reports/96072/index.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?sa=t&amp;source=web&amp;rct=j&amp;opi=89978449&amp;url=http://www.famsi.org/reports/01051/pmed.pdf&amp;ved=2ahUKEwi2ncvx0OGKAxXZ48kDHRRpCtYQFnoECBIQAQ&amp;usg=AOvVaw0b8K26ssoz8VBqJ7Ud78qo</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Norman, OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,17 +379,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,33 +671,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -512,169 +711,516 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F2" s="1">
+        <v>1532</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>384</v>
+      </c>
+      <c r="H4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2003</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1532</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2001</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2010</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="1">
-        <v>384</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{EA4E9817-F41C-4ACE-929C-D6F80F529CD5}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{92DEA5EA-82B8-4E20-8FBD-F584580110E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>